<commit_message>
Update heating and budget
</commit_message>
<xml_diff>
--- a/000house/20140216 Porch and Master Bath/Contractors/Contractors.xlsx
+++ b/000house/20140216 Porch and Master Bath/Contractors/Contractors.xlsx
@@ -4,23 +4,24 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="225" windowWidth="14805" windowHeight="7890" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="285" windowWidth="14805" windowHeight="6900" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="GC" sheetId="1" r:id="rId1"/>
     <sheet name="Subs" sheetId="2" r:id="rId2"/>
-    <sheet name="Plumbing" sheetId="3" r:id="rId3"/>
-    <sheet name="GCcandidates" sheetId="4" r:id="rId4"/>
+    <sheet name="Electrical" sheetId="5" r:id="rId3"/>
+    <sheet name="Plumbing" sheetId="3" r:id="rId4"/>
+    <sheet name="GCcandidates" sheetId="4" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Subs!$A$1:$K$21</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Subs!$A$1:$L$23</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="279">
   <si>
     <t>Apergis</t>
   </si>
@@ -514,9 +515,6 @@
     <t>Wilcox Electric</t>
   </si>
   <si>
-    <t>w: 202-546-1010</t>
-  </si>
-  <si>
     <t>Aspen Hill Plumbing</t>
   </si>
   <si>
@@ -621,10 +619,6 @@
   <si>
     <t>12/5: Contacted by email. Briefly described project and asked for a bid.
 12/5: Declined. Too busy.</t>
-  </si>
-  <si>
-    <t>12/5: Contacted via Wilcox business website. Briefly described project and asked for a bid.
-12/7: Called and set up a site visit for Dec 28 between 11:30 and 12:30.</t>
   </si>
   <si>
     <t>Angie's list (A; 294 reviews)</t>
@@ -762,65 +756,10 @@
 12/21: Merrick lowered price to $24,600 or $21,500 (I buy lights and bath fans).</t>
   </si>
   <si>
-    <t>12/17: Doug put us in contact. We agreed to meet Friday 12/18 at 2pm. I sent email with plans.
-12/18: We will meet 12/28 at 9:30</t>
-  </si>
-  <si>
-    <t>12/9: Called. Priced the disconnect of 2 AC units at $500. Arranged the job for Friday at 10am. We will discuss rest of project.</t>
-  </si>
-  <si>
-    <t>12/10: Shawn Mullan called asked if he could come early, 9am.</t>
-  </si>
-  <si>
-    <t>12/11: Shawn arrived 10 minutes early and completed disconnect in 1 hour. Started to discuss rest of project and he said I should talk to his father-in-law Bob, furnace expert. Sent drawings and rfp.</t>
-  </si>
-  <si>
-    <t>12/15: Had not heard anything. Called to see if interested. Agreed on site visit on Wed 12/16 around 4pm. Need to deal with drain in foundation.</t>
-  </si>
-  <si>
-    <t>12/16: Site visit went well. He will be able to do the project. Asked for me to send building permit #. Asked me to talk to 3rd party inspector about area drain (to sewer or to sump). He will send an estimate.</t>
-  </si>
-  <si>
-    <t>12/17: Sent building permit number. Began relationship with inspector. Need to talk to inspector. Received estimate of project $3000.</t>
-  </si>
-  <si>
-    <t>12/18: Made plan with plumber and paid him $1500 deposit.</t>
-  </si>
-  <si>
-    <t>12/23: Change of plans. Use existing area drain. No plumbing now.</t>
-  </si>
-  <si>
-    <t>12/27: Asked Bob to visit Tuesday when drains exposed for concrete. Asked for receipts ($500, $1500). Asked for estimates (plumbing, heating).</t>
-  </si>
-  <si>
     <t>Bob Gable</t>
   </si>
   <si>
     <t>GC notes</t>
-  </si>
-  <si>
-    <t>12/27: Concrete entry way, closet, and steps should be ready for concrete on Wednesday 12/30. Plumber will hopefully visit Tuesday. I asked if Oscar needed an inspection.</t>
-  </si>
-  <si>
-    <t>12/22: Inspector returned and passed us for concrete footings.</t>
-  </si>
-  <si>
-    <t>12/24: North wall of back entry wall too tall. We will talk about it on Satuday 12/26</t>
-  </si>
-  <si>
-    <t>12/26: Met with Oscar and wall is being reduced. We talked about dirt being used to regrade sloping corner of yard. Oscar said he would do it.</t>
-  </si>
-  <si>
-    <t>12/26: I asked that I have a chance to request privacy windows for the master bath.</t>
-  </si>
-  <si>
-    <t>12/26: Oscar offered to put me in touch with his electrician. We also visited SPRC about the columns.</t>
-  </si>
-  <si>
-    <t>12/26: I asked that AC lines be cut and that the copper be saved for scrap sale. Oscar said ok.</t>
-  </si>
-  <si>
-    <t>12/27: Follow up email on items from 12/26.</t>
   </si>
   <si>
     <t>12/5: Called late, no answer. Sent email describing project and including plans. Invited for a visit and to submit a bid.
@@ -828,6 +767,175 @@
 12/8: Dave confirmed. He will call with 30 min ETA.
 12/14: Site visit went well. Suggested keep the stack outside to the existing (to be moved) drain. Same with drain for utility sink. Also suggested to keep heating system simple. Will send estimate by the end of the week. Does not believe can do the work before the new year.
 12/18: Dave gave estimates. Ground work and general remodel plumbing $25,750, hot water recirculating system $1850, in floor radiant heating $13,720, runtall radiators $23,040</t>
+  </si>
+  <si>
+    <t>Wilcox</t>
+  </si>
+  <si>
+    <t>Steve</t>
+  </si>
+  <si>
+    <t>crystal@wilcox-electric.com</t>
+  </si>
+  <si>
+    <t>w: 202-546-1010
+w: 301-583-8888
+m: 202-664-4023</t>
+  </si>
+  <si>
+    <t>12/17: Doug put us in contact. We agreed to meet Friday 12/18 at 2pm. I sent email with plans.
+12/18: We will meet 12/28 at 9:30
+12/28: Eric forgot. I called him and he came quickly. We reviewed the job. He did not believe that the panel needed to be moved. He will put together a proposal in about a week. NOT AN ELECTRICIAN. Associated with licensed electrician Larry from Advanced Construction. 240-752-2588</t>
+  </si>
+  <si>
+    <t>12/5: Contacted via Wilcox business website. Briefly described project and asked for a bid.
+12/7: Called and set up a site visit for Dec 28 between 11:30 and 12:30.
+12/28: Steve Wilcox arrived. We reviewed the project. He thought the panel needed to be moved or the hot water heater needed to be moved. He will put together a proposal in about a week. He asked me to email plans, which I did.</t>
+  </si>
+  <si>
+    <t>McKevitt</t>
+  </si>
+  <si>
+    <t>Justin</t>
+  </si>
+  <si>
+    <t>HVAC/Plumbing</t>
+  </si>
+  <si>
+    <t>m: 240-527-0569</t>
+  </si>
+  <si>
+    <t>FDA: Bobby Thompson</t>
+  </si>
+  <si>
+    <t>Lopez</t>
+  </si>
+  <si>
+    <t>Rudy</t>
+  </si>
+  <si>
+    <t>JBR Electric, LLC</t>
+  </si>
+  <si>
+    <t>jbrrudylopez@yahoo.com</t>
+  </si>
+  <si>
+    <t>m: 301-537-3714</t>
+  </si>
+  <si>
+    <t>Rudy Lopez</t>
+  </si>
+  <si>
+    <t>Concrete on track for inspection Wed afternoon. Plumbing and electrical related to concrete in back should be also be ready. Discussed grading back yard. Remove timbers of raised garden. Add 6x6 timbers with dead men as a retaining wall in front of fence. Add rain leader from house to drain into retaining wall outside fence, which has a drain.</t>
+  </si>
+  <si>
+    <t>Concrete entry way, closet, and steps should be ready for concrete on Wednesday 12/30. Plumber will hopefully visit Tuesday. I asked if Oscar needed an inspection.</t>
+  </si>
+  <si>
+    <t>Follow up email on items from 12/26.</t>
+  </si>
+  <si>
+    <t>Met with Oscar and wall is being reduced. We talked about dirt being used to regrade sloping corner of yard. Oscar said he would do it.</t>
+  </si>
+  <si>
+    <t>I asked that I have a chance to request privacy windows for the master bath.</t>
+  </si>
+  <si>
+    <t>Oscar offered to put me in touch with his electrician. We also visited SPRC about the columns.</t>
+  </si>
+  <si>
+    <t>I asked that AC lines be cut and that the copper be saved for scrap sale. Oscar said ok.</t>
+  </si>
+  <si>
+    <t>North wall of back entry wall too tall. We will talk about it on Satuday 12/26</t>
+  </si>
+  <si>
+    <t>Inspector returned and passed us for concrete footings.</t>
+  </si>
+  <si>
+    <t>Oscar Flores sent Rudy to visit. He can do the job for $14,900, not sure about fixtures, coax/ethernet. I said lets do it. He will do rough-out for sconces at steps in back right away.</t>
+  </si>
+  <si>
+    <t>Asked Bob to visit Tuesday when drains exposed for concrete. Asked for receipts ($500, $1500). Asked for estimates (plumbing, heating).</t>
+  </si>
+  <si>
+    <t>Change of plans. Use existing area drain. No plumbing now.</t>
+  </si>
+  <si>
+    <t>Made plan with plumber and paid him $1500 deposit.</t>
+  </si>
+  <si>
+    <t>Sent building permit number. Began relationship with inspector. Need to talk to inspector. Received estimate of project $3000.</t>
+  </si>
+  <si>
+    <t>Site visit went well. He will be able to do the project. Asked for me to send building permit #. Asked me to talk to 3rd party inspector about area drain (to sewer or to sump). He will send an estimate.</t>
+  </si>
+  <si>
+    <t>Had not heard anything. Called to see if interested. Agreed on site visit on Wed 12/16 around 4pm. Need to deal with drain in foundation.</t>
+  </si>
+  <si>
+    <t>Shawn arrived 10 minutes early and completed disconnect in 1 hour. Started to discuss rest of project and he said I should talk to his father-in-law Bob, furnace expert. Sent drawings and rfp.</t>
+  </si>
+  <si>
+    <t>Shawn Mullan called asked if he could come early, 9am.</t>
+  </si>
+  <si>
+    <t>Called. Priced the disconnect of 2 AC units at $500. Arranged the job for Friday at 10am. We will discuss rest of project.</t>
+  </si>
+  <si>
+    <t>contatct date</t>
+  </si>
+  <si>
+    <t>Bob visited. We decided to cut and cap the drain from the gutters. He will do Wed am 12/30. We talked about moving water heater options and also talked about replacing boiler with condenser boiler/hot water heater combo. He sent brochure. It is small and can go anywhere. He will get me an estimate on the main plumbing job for the new bathrooms. He will get me receipts for work.</t>
+  </si>
+  <si>
+    <t>Researched 96,000 BTU Output Challenger Combo Boiler - Space Heating &amp; Domestic Hot Water (condensing)
+SKU:CC-125, Brand: Triangle Tube. It costs $2659.95. Replace existing is top option.</t>
+  </si>
+  <si>
+    <t>Bob cut and capped original drain from gutters.</t>
+  </si>
+  <si>
+    <t>Inspector came and passed our foundation/slab at back exit. He said replacing boiler and HW with small combo unit was a good idea. Eliminate conflicts with existing panel. Cement not coming until Monday. We discussed demo chimney instead of repair and extend: even swap. Proposal for church work coming tomorrow morning.</t>
+  </si>
+  <si>
+    <t>Discussed adding a sub-panel on the third floor instead of new panel in basement. Hoped for a discoung.</t>
+  </si>
+  <si>
+    <t>Can't start today. On another job. He will be ready for cement on Monday. He will install phone/coax/ethernet offsetting cost bonus of the sub-panel approach.</t>
+  </si>
+  <si>
+    <t>Otvos</t>
+  </si>
+  <si>
+    <t>Peter</t>
+  </si>
+  <si>
+    <t>WarmBoard</t>
+  </si>
+  <si>
+    <t>In-floor radiant heating</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> potvos@warmboard.com</t>
+  </si>
+  <si>
+    <t>w: 831-219-1036</t>
+  </si>
+  <si>
+    <t>Began proposal process. Shared drawings pdf and gross estimates ($7.59 -Structural, $6.99 -Retrofit). Next steps: cad files ($200 fee if pdf), design ($500), and design questions.</t>
+  </si>
+  <si>
+    <t>Ahmann</t>
+  </si>
+  <si>
+    <t>Found Bosch unit. Better gpm for hot water. Name brand for parts and service. ZWB28-3. Asked for estimates related to boiler (remove existing, install new, servew new batrooms, in-floor radiant heating) and bathrooms. Asked to talk about details.</t>
+  </si>
+  <si>
+    <t>Bob replied. $7000 to install combo boiler/dhw and $12000 for bathrooms.</t>
+  </si>
+  <si>
+    <t>I said let's do Bosch. Asked when and how long it will take. I asked to talk about details. Bob called later and we talked about details. I will cc him when I email warmboard supplier.</t>
   </si>
 </sst>
 </file>
@@ -896,7 +1004,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -916,26 +1024,54 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1239,86 +1375,130 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A9"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F1" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A3" sqref="A3"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="14.28515625" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125" customWidth="1"/>
-    <col min="6" max="6" width="37" customWidth="1"/>
-    <col min="8" max="8" width="30.42578125" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" style="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="100.7109375" style="25" customWidth="1"/>
+    <col min="3" max="5" width="14.28515625" style="11" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" style="11" customWidth="1"/>
+    <col min="7" max="7" width="37" style="11" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" style="11"/>
+    <col min="9" max="9" width="30.42578125" style="11" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2" s="24">
+        <v>42368</v>
+      </c>
+      <c r="B2" s="25" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A3" s="13">
+        <v>42367</v>
+      </c>
+      <c r="B3" s="25" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="13">
+        <v>42365</v>
+      </c>
+      <c r="B4" s="25" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>237</v>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="13">
+        <v>42365</v>
+      </c>
+      <c r="B5" s="25" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="13">
+        <v>42364</v>
+      </c>
+      <c r="B6" s="25" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="13">
+        <v>42364</v>
+      </c>
+      <c r="B7" s="25" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="13">
+        <v>42364</v>
+      </c>
+      <c r="B8" s="25" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="13">
+        <v>42364</v>
+      </c>
+      <c r="B9" s="25" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="13">
+        <v>42362</v>
+      </c>
+      <c r="B10" s="25" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="13">
+        <v>42360</v>
+      </c>
+      <c r="B11" s="25" t="s">
+        <v>250</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:O11">
-    <sortCondition descending="1" ref="A2:A11"/>
+  <sortState ref="B2:P11">
+    <sortCondition descending="1" ref="B2:B11"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="72" orientation="portrait" r:id="rId1"/>
+  <colBreaks count="1" manualBreakCount="1">
+    <brk id="2" max="9" man="1"/>
+  </colBreaks>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N21"/>
+  <dimension ref="A1:O24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="G8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="I8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H10" sqref="H10"/>
+      <selection pane="bottomRight" activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1327,14 +1507,15 @@
     <col min="4" max="5" width="18.7109375" style="5" customWidth="1"/>
     <col min="6" max="6" width="31.42578125" style="5" customWidth="1"/>
     <col min="7" max="7" width="15.140625" style="5" customWidth="1"/>
-    <col min="8" max="8" width="37" style="9" customWidth="1"/>
-    <col min="9" max="9" width="37" style="5" customWidth="1"/>
-    <col min="10" max="10" width="10.5703125" style="5" customWidth="1"/>
-    <col min="11" max="11" width="18.140625" style="5" customWidth="1"/>
-    <col min="12" max="14" width="9.140625" style="5"/>
+    <col min="8" max="8" width="11.7109375" style="18" customWidth="1"/>
+    <col min="9" max="9" width="37" style="18" customWidth="1"/>
+    <col min="10" max="10" width="37" style="5" customWidth="1"/>
+    <col min="11" max="11" width="11.7109375" style="5" customWidth="1"/>
+    <col min="12" max="12" width="18.140625" style="5" customWidth="1"/>
+    <col min="13" max="15" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="B1" s="5" t="s">
         <v>6</v>
       </c>
@@ -1353,46 +1534,49 @@
       <c r="G1" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="18" t="s">
+        <v>261</v>
+      </c>
+      <c r="I1" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="D2" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="F2" s="7" t="s">
         <v>216</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="G2" s="5" t="s">
         <v>217</v>
       </c>
-      <c r="F2" s="7" t="s">
-        <v>218</v>
-      </c>
-      <c r="G2" s="5" t="s">
+      <c r="I2" s="18" t="s">
         <v>219</v>
       </c>
-      <c r="H2" s="9" t="s">
-        <v>221</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>222</v>
-      </c>
       <c r="J2" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="K2" s="5" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1400,590 +1584,668 @@
         <v>89</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F3" s="7"/>
       <c r="G3" s="5" t="s">
-        <v>220</v>
-      </c>
-      <c r="J3" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="K3" s="5" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>119</v>
       </c>
       <c r="F4" s="7"/>
       <c r="G4" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="H4" s="15" t="str">
-        <f>(Plumbing!A3)</f>
-        <v>12/27: Asked Bob to visit Tuesday when drains exposed for concrete. Asked for receipts ($500, $1500). Asked for estimates (plumbing, heating).</v>
-      </c>
-      <c r="I4" s="5" t="s">
-        <v>200</v>
+        <v>208</v>
+      </c>
+      <c r="H4" s="19">
+        <f>Plumbing!$A$8</f>
+        <v>42367</v>
+      </c>
+      <c r="I4" s="10" t="str">
+        <f>(Plumbing!$B$3)</f>
+        <v>I said let's do Bosch. Asked when and how long it will take. I asked to talk about details. Bob called later and we talked about details. I will cc him when I email warmboard supplier.</v>
       </c>
       <c r="J4" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="K4" s="5" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>119</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>209</v>
-      </c>
-      <c r="H5" s="15"/>
-    </row>
-    <row r="6" spans="1:11" ht="315" x14ac:dyDescent="0.25">
+        <v>207</v>
+      </c>
+      <c r="H5" s="19"/>
+      <c r="I5" s="10"/>
+    </row>
+    <row r="6" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>138</v>
+        <v>236</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>139</v>
+        <v>237</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>130</v>
+        <v>238</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>140</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>143</v>
+        <v>239</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="H6" s="11" t="s">
-        <v>223</v>
-      </c>
-      <c r="J6" s="5" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+        <v>240</v>
+      </c>
+      <c r="H6" s="19">
+        <f>Electrical!$A$5</f>
+        <v>42367</v>
+      </c>
+      <c r="I6" s="10" t="str">
+        <f>Electrical!$B$5</f>
+        <v>Oscar Flores sent Rudy to visit. He can do the job for $14,900, not sure about fixtures, coax/ethernet. I said lets do it. He will do rough-out for sconces at steps in back right away.</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>268</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>269</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>150</v>
+        <v>270</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>140</v>
-      </c>
-      <c r="F7" s="7"/>
+        <v>271</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>272</v>
+      </c>
       <c r="G7" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="H7" s="11" t="s">
-        <v>186</v>
-      </c>
-      <c r="I7" s="5" t="s">
-        <v>161</v>
-      </c>
-      <c r="J7" s="5" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+        <v>273</v>
+      </c>
+      <c r="H7" s="19">
+        <v>42369</v>
+      </c>
+      <c r="I7" s="10" t="s">
+        <v>274</v>
+      </c>
+      <c r="K7" s="5" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="315" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>212</v>
+        <v>138</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>213</v>
+        <v>139</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>130</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>140</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>214</v>
+        <v>143</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>215</v>
-      </c>
-      <c r="H8" s="11" t="s">
-        <v>224</v>
-      </c>
-      <c r="J8" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="I8" s="20" t="s">
+        <v>221</v>
+      </c>
+      <c r="K8" s="5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="180" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>2</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>225</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>227</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="I9" s="20" t="s">
+        <v>230</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="K9" s="5" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="180" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>2</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="I10" s="20" t="s">
+        <v>229</v>
+      </c>
+      <c r="K10" s="5" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="330" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>3</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>182</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>183</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>152</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>153</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>154</v>
-      </c>
-      <c r="G9" s="5" t="s">
-        <v>211</v>
-      </c>
-      <c r="H9" s="11" t="s">
-        <v>244</v>
-      </c>
-      <c r="I9" s="5" t="s">
-        <v>160</v>
-      </c>
-      <c r="J9" s="5" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" ht="135" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>3</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>201</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>202</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>180</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>205</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>204</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>203</v>
-      </c>
-      <c r="H10" s="11" t="s">
-        <v>206</v>
-      </c>
-      <c r="I10" s="5" t="s">
-        <v>189</v>
-      </c>
-      <c r="J10" s="5" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" ht="330" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>3</v>
       </c>
       <c r="B11" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="I11" s="20" t="s">
+        <v>224</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="K11" s="5" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="135" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>3</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="I12" s="21" t="s">
+        <v>204</v>
+      </c>
+      <c r="J12" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="K12" s="5" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>3</v>
+      </c>
+      <c r="B13" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C13" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D13" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="E13" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="F11" s="7" t="s">
+      <c r="F13" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="G11" s="5" t="s">
+      <c r="G13" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="I11" s="5" t="s">
+      <c r="J13" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="J11" s="5" t="s">
+      <c r="K13" s="5" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="255" x14ac:dyDescent="0.25">
-      <c r="A12">
+    <row r="14" spans="1:12" ht="255" x14ac:dyDescent="0.25">
+      <c r="A14">
         <v>10</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B14" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C14" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D14" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="E14" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="F12" s="7" t="s">
+      <c r="F14" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="G12" s="5" t="s">
+      <c r="G14" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="H12" s="11" t="s">
+      <c r="I14" s="20" t="s">
         <v>142</v>
       </c>
-      <c r="J12" s="5" t="s">
+      <c r="K14" s="5" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="105" x14ac:dyDescent="0.25">
-      <c r="B13" s="5" t="s">
+    <row r="15" spans="1:12" ht="105" x14ac:dyDescent="0.25">
+      <c r="B15" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C15" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D15" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="E15" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="F13" s="7" t="s">
+      <c r="F15" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="G13" s="5" t="s">
+      <c r="G15" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="H13" s="10" t="s">
+      <c r="I15" s="22" t="s">
         <v>107</v>
       </c>
-      <c r="I13" s="5" t="s">
+      <c r="J15" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="J13" s="5" t="s">
+      <c r="K15" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="K13" s="5" t="s">
+      <c r="L15" s="5" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="210" x14ac:dyDescent="0.25">
-      <c r="B14" s="5" t="s">
+    <row r="16" spans="1:12" ht="210" x14ac:dyDescent="0.25">
+      <c r="B16" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C16" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D16" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="E14" s="5" t="s">
+      <c r="E16" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="F14" s="7" t="s">
+      <c r="F16" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="G14" s="5" t="s">
+      <c r="G16" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="H14" s="14" t="s">
+      <c r="I16" s="22" t="s">
         <v>122</v>
       </c>
-      <c r="I14" s="5" t="s">
+      <c r="J16" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="J14" s="5" t="s">
+      <c r="K16" s="5" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="B15" s="5" t="s">
+    <row r="17" spans="2:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="B17" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C17" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D17" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="E15" s="5" t="s">
+      <c r="E17" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="F15" s="7" t="s">
+      <c r="F17" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="G15" s="5" t="s">
+      <c r="G17" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="H15" s="9" t="s">
+      <c r="I17" s="18" t="s">
         <v>105</v>
       </c>
-      <c r="I15" s="5" t="s">
+      <c r="J17" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="J15" s="5" t="s">
+      <c r="K17" s="5" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="120" x14ac:dyDescent="0.25">
-      <c r="B16" s="5" t="s">
+    <row r="18" spans="2:11" ht="120" x14ac:dyDescent="0.25">
+      <c r="B18" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C18" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="E16" s="5" t="s">
+      <c r="E18" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="F16" s="7" t="s">
+      <c r="F18" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="G16" s="5" t="s">
+      <c r="G18" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="H16" s="14" t="s">
+      <c r="I18" s="22" t="s">
         <v>123</v>
       </c>
-      <c r="J16" s="5" t="s">
+      <c r="K18" s="5" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="17" spans="2:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="D17" s="5" t="s">
+    <row r="19" spans="2:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="D19" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="E19" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="E17" s="5" t="s">
+      <c r="F19" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="F17" s="7" t="s">
+      <c r="G19" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="I19" s="22" t="s">
+        <v>193</v>
+      </c>
+      <c r="J19" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="G17" s="5" t="s">
+      <c r="K19" s="5" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="B20" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="I20" s="22" t="s">
+        <v>191</v>
+      </c>
+      <c r="K20" s="5" t="s">
         <v>173</v>
       </c>
-      <c r="H17" s="14" t="s">
-        <v>195</v>
-      </c>
-      <c r="I17" s="5" t="s">
+    </row>
+    <row r="21" spans="2:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="D21" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="F21" s="7"/>
+      <c r="G21" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="I21" s="22" t="s">
+        <v>190</v>
+      </c>
+      <c r="J21" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="K21" s="5" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="22" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="B22" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="F22" s="7"/>
+      <c r="G22" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="I22" s="23"/>
+    </row>
+    <row r="23" spans="2:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="B23" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="I23" s="21" t="s">
+        <v>184</v>
+      </c>
+      <c r="K23" s="5" t="s">
         <v>158</v>
       </c>
-      <c r="J17" s="5" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="18" spans="2:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="B18" s="5" t="s">
-        <v>167</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>169</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>170</v>
-      </c>
-      <c r="F18" s="7" t="s">
-        <v>171</v>
-      </c>
-      <c r="G18" s="5" t="s">
-        <v>172</v>
-      </c>
-      <c r="H18" s="14" t="s">
-        <v>193</v>
-      </c>
-      <c r="J18" s="5" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="19" spans="2:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="D19" s="5" t="s">
-        <v>175</v>
-      </c>
-      <c r="E19" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="F19" s="7"/>
-      <c r="G19" s="5" t="s">
-        <v>176</v>
-      </c>
-      <c r="H19" s="14" t="s">
-        <v>192</v>
-      </c>
-      <c r="I19" s="5" t="s">
-        <v>190</v>
-      </c>
-      <c r="J19" s="5" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="20" spans="2:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B20" s="5" t="s">
-        <v>177</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>178</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>179</v>
-      </c>
-      <c r="F20" s="7"/>
-      <c r="G20" s="5" t="s">
-        <v>181</v>
-      </c>
-      <c r="H20" s="13"/>
-    </row>
-    <row r="21" spans="2:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="B21" s="5" t="s">
-        <v>162</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>163</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>164</v>
-      </c>
-      <c r="E21" s="5" t="s">
-        <v>140</v>
-      </c>
-      <c r="F21" s="7" t="s">
-        <v>166</v>
-      </c>
-      <c r="G21" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="H21" s="10" t="s">
-        <v>185</v>
-      </c>
-      <c r="J21" s="5" t="s">
-        <v>159</v>
+    </row>
+    <row r="24" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="B24" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>232</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="G24" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="K24" s="5" t="s">
+        <v>235</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K21">
+  <autoFilter ref="A1:L23">
     <sortState ref="A2:K21">
       <sortCondition ref="A1:A21"/>
     </sortState>
   </autoFilter>
   <hyperlinks>
-    <hyperlink ref="F13" r:id="rId1" display="edyleonel2013@gmail.com"/>
-    <hyperlink ref="F14" r:id="rId2"/>
-    <hyperlink ref="F15" r:id="rId3"/>
-    <hyperlink ref="F16" r:id="rId4"/>
-    <hyperlink ref="F12" r:id="rId5"/>
-    <hyperlink ref="F11" r:id="rId6"/>
-    <hyperlink ref="F6" r:id="rId7" display="merrickbes@gmail.com"/>
-    <hyperlink ref="F9" r:id="rId8"/>
-    <hyperlink ref="F17" r:id="rId9"/>
-    <hyperlink ref="F21" r:id="rId10"/>
-    <hyperlink ref="F18" r:id="rId11"/>
-    <hyperlink ref="F10" r:id="rId12" display="sales@rbincorporated.com"/>
-    <hyperlink ref="F8" r:id="rId13"/>
+    <hyperlink ref="F15" r:id="rId1" display="edyleonel2013@gmail.com"/>
+    <hyperlink ref="F16" r:id="rId2"/>
+    <hyperlink ref="F17" r:id="rId3"/>
+    <hyperlink ref="F18" r:id="rId4"/>
+    <hyperlink ref="F14" r:id="rId5"/>
+    <hyperlink ref="F13" r:id="rId6"/>
+    <hyperlink ref="F8" r:id="rId7" display="merrickbes@gmail.com"/>
+    <hyperlink ref="F11" r:id="rId8"/>
+    <hyperlink ref="F19" r:id="rId9"/>
+    <hyperlink ref="F23" r:id="rId10"/>
+    <hyperlink ref="F20" r:id="rId11"/>
+    <hyperlink ref="F12" r:id="rId12" display="sales@rbincorporated.com"/>
+    <hyperlink ref="F10" r:id="rId13"/>
     <hyperlink ref="F2" r:id="rId14"/>
+    <hyperlink ref="F9" r:id="rId15"/>
+    <hyperlink ref="F6" r:id="rId16"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId15"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId17"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A11"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" style="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="100.7109375" style="16" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>225</v>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="15" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="17">
+        <v>42368</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="17">
+        <v>42367</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="17">
+        <v>42367</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>251</v>
       </c>
     </row>
   </sheetData>
@@ -1992,6 +2254,155 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" style="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="100.7109375" style="16" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="15" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="17">
+        <v>42372</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="17">
+        <v>42372</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="17">
+        <v>42370</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="17">
+        <v>42368</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="17">
+        <v>42368</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A8" s="17">
+        <v>42367</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="17">
+        <v>42365</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="17">
+        <v>42361</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="17">
+        <v>42356</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="17">
+        <v>42355</v>
+      </c>
+      <c r="B12" s="16" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="17">
+        <v>42354</v>
+      </c>
+      <c r="B13" s="16" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="17">
+        <v>42353</v>
+      </c>
+      <c r="B14" s="16" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="17">
+        <v>42349</v>
+      </c>
+      <c r="B15" s="16" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="17">
+        <v>42348</v>
+      </c>
+      <c r="B16" s="16" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="17">
+        <v>42347</v>
+      </c>
+      <c r="B17" s="16" t="s">
+        <v>260</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O13"/>
   <sheetViews>
@@ -2407,7 +2818,7 @@
       <c r="E10" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="F10" s="12"/>
+      <c r="F10" s="9"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11">

</xml_diff>

<commit_message>
added special inspections and on site inspection report
</commit_message>
<xml_diff>
--- a/000house/20140216 Porch and Master Bath/Contractors/Contractors.xlsx
+++ b/000house/20140216 Porch and Master Bath/Contractors/Contractors.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="285" windowWidth="14805" windowHeight="6900" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="285" windowWidth="14805" windowHeight="6900" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="GC" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="292">
   <si>
     <t>Apergis</t>
   </si>
@@ -895,9 +895,6 @@
     <t>Ahmann</t>
   </si>
   <si>
-    <t>Found Bosch unit. Better gpm for hot water. Name brand for parts and service. ZWB28-3. Asked for estimates related to boiler (remove existing, install new, servew new batrooms, in-floor radiant heating) and bathrooms. Asked to talk about details.</t>
-  </si>
-  <si>
     <t>Bob replied. $7000 to install combo boiler/dhw and $12000 for bathrooms.</t>
   </si>
   <si>
@@ -965,6 +962,25 @@
   </si>
   <si>
     <t>contact date</t>
+  </si>
+  <si>
+    <t>Installed Triangle tube challenger $7000 ($2700 appliance).</t>
+  </si>
+  <si>
+    <t>Receipt received. System not operating properly. Bob revisited bled the air out of system.</t>
+  </si>
+  <si>
+    <t>System still not operating properly… too hot. Bob stopped by and installed outdoor reset control (via exterior thermostat).</t>
+  </si>
+  <si>
+    <t>System still not operating properly… too cold. Bob will visit on Monday to "fine tune".</t>
+  </si>
+  <si>
+    <t>Bob visited. He diagnoses the problem as the thermostat. We need one with zero residual voltage. We have one with some low residual voltage.</t>
+  </si>
+  <si>
+    <t>Found Bosch unit. Better gpm for hot water. Name brand for parts and service. ZWB28-3. Asked for estimates related to boiler (remove existing, install new, servew new batrooms, in-floor radiant heating) and bathrooms. Asked to talk about details. 
+Bosch Greenstar ZWB28-3A23, module IPM2 for two heating zones and mixing capability, optional concentric vent kit for horizontal direct vent</t>
   </si>
 </sst>
 </file>
@@ -1520,11 +1536,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I4" sqref="I4"/>
+      <selection pane="bottomRight" activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1561,7 +1577,7 @@
         <v>69</v>
       </c>
       <c r="H1" s="18" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="I1" s="18" t="s">
         <v>73</v>
@@ -1581,10 +1597,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>282</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>283</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>284</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>214</v>
@@ -1613,7 +1629,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>89</v>
@@ -1625,7 +1641,7 @@
         <v>215</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="G3" s="5" t="s">
         <v>218</v>
@@ -1655,12 +1671,12 @@
         <v>208</v>
       </c>
       <c r="H4" s="19">
-        <f>Plumbing!$A$9</f>
-        <v>42367</v>
+        <f>Plumbing!$A$3</f>
+        <v>42380</v>
       </c>
       <c r="I4" s="10" t="str">
         <f>(Plumbing!$B$3)</f>
-        <v>Bob gave his recommendation after reading the manuals for the Bosch and Triangle Tube. He recommended Triangle Tube. I said ok. He will get started. Parts delivered in about a week. Install in one day.</v>
+        <v>Bob visited. He diagnoses the problem as the thermostat. We need one with zero residual voltage. We have one with some low residual voltage.</v>
       </c>
       <c r="J4" s="5" t="s">
         <v>198</v>
@@ -1725,7 +1741,7 @@
         <v>We reviewed proposal and my addendum, signed it, and I paid 50%. Rudy will rough out the electrical for the cement today, get the permit, and get started on the rough out for the new service location.</v>
       </c>
       <c r="K6" s="5" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="165" x14ac:dyDescent="0.25">
@@ -1754,7 +1770,7 @@
         <v>42373</v>
       </c>
       <c r="I7" s="10" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="K7" s="5" t="s">
         <v>269</v>
@@ -1783,7 +1799,7 @@
         <v>141</v>
       </c>
       <c r="I8" s="21" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="K8" s="5" t="s">
         <v>101</v>
@@ -1812,7 +1828,7 @@
         <v>226</v>
       </c>
       <c r="I9" s="21" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="J9" s="5" t="s">
         <v>160</v>
@@ -1841,7 +1857,7 @@
         <v>213</v>
       </c>
       <c r="I10" s="21" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="K10" s="5" t="s">
         <v>91</v>
@@ -1870,7 +1886,7 @@
         <v>209</v>
       </c>
       <c r="I11" s="21" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="J11" s="5" t="s">
         <v>159</v>
@@ -2269,7 +2285,7 @@
         <v>42374</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -2277,7 +2293,7 @@
         <v>42373</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -2311,10 +2327,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:B23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2335,129 +2351,169 @@
     </row>
     <row r="3" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="17">
+        <v>42380</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="17">
+        <v>42379</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="17">
+        <v>42378</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="17">
+        <v>42377</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="17">
+        <v>42376</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="17">
         <v>42373</v>
       </c>
-      <c r="B3" s="16" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="17">
+      <c r="B8" s="16" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="17">
         <v>42372</v>
       </c>
-      <c r="B4" s="16" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="17">
+      <c r="B9" s="16" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="17">
         <v>42372</v>
       </c>
-      <c r="B5" s="16" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="17">
+      <c r="B10" s="16" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A11" s="17">
         <v>42370</v>
       </c>
-      <c r="B6" s="16" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="17">
+      <c r="B11" s="16" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="17">
         <v>42368</v>
       </c>
-      <c r="B7" s="16" t="s">
+      <c r="B12" s="16" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="17">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="17">
         <v>42368</v>
       </c>
-      <c r="B8" s="16" t="s">
+      <c r="B13" s="16" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A9" s="17">
+    <row r="14" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A14" s="17">
         <v>42367</v>
       </c>
-      <c r="B9" s="16" t="s">
+      <c r="B14" s="16" t="s">
         <v>257</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="17">
-        <v>42365</v>
-      </c>
-      <c r="B10" s="16" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="17">
-        <v>42361</v>
-      </c>
-      <c r="B11" s="16" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="17">
-        <v>42356</v>
-      </c>
-      <c r="B12" s="16" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="17">
-        <v>42355</v>
-      </c>
-      <c r="B13" s="16" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="17">
-        <v>42354</v>
-      </c>
-      <c r="B14" s="16" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="17">
-        <v>42353</v>
+        <v>42365</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="17">
-        <v>42349</v>
+        <v>42361</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="17">
-        <v>42348</v>
+        <v>42356</v>
       </c>
       <c r="B17" s="16" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="17">
+        <v>42355</v>
+      </c>
+      <c r="B18" s="16" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="17">
+        <v>42354</v>
+      </c>
+      <c r="B19" s="16" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="17">
+        <v>42353</v>
+      </c>
+      <c r="B20" s="16" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="17">
+        <v>42349</v>
+      </c>
+      <c r="B21" s="16" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="17">
+        <v>42348</v>
+      </c>
+      <c r="B22" s="16" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="17">
         <v>42347</v>
       </c>
-      <c r="B18" s="16" t="s">
+      <c r="B23" s="16" t="s">
         <v>256</v>
       </c>
     </row>

</xml_diff>